<commit_message>
Rj local mapping states data to wa de (#316)
* Mnwr update
</commit_message>
<xml_diff>
--- a/2_CodeMappingTemplates/WaterAllocation_WaterUse/XX_Allocation and Water Use Schema Mapping to WaDE.xlsx
+++ b/2_CodeMappingTemplates/WaterAllocation_WaterUse/XX_Allocation and Water Use Schema Mapping to WaDE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\California\WaterAllocation_WaterUse_CSWRCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\2_CodeMappingTemplates\WaterAllocation_WaterUse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303376EF-A9A5-41FC-BBB6-2F2321748C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2ED81F-90F8-4360-A507-2E1DB4114991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="645" activeTab="8" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="645" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="345">
   <si>
     <t>Name</t>
   </si>
@@ -1056,6 +1056,27 @@
   <si>
     <t>Refers back to the state URL that describes the water right (e.g., https://www.waterrights.utah.gov/asp_apps/wrprint/wrprint.asp?wrnum=55-12888).</t>
   </si>
+  <si>
+    <t>*get from sites.csv</t>
+  </si>
+  <si>
+    <t>XXwr_WR + AllocationNativeID</t>
+  </si>
+  <si>
+    <t>XXwr_M1</t>
+  </si>
+  <si>
+    <t>XXwr_O1</t>
+  </si>
+  <si>
+    <t>XXwr_V1</t>
+  </si>
+  <si>
+    <t>XXwr_WS + WaterSourceNativeID</t>
+  </si>
+  <si>
+    <t>XXwr_S + SiteNativeID</t>
+  </si>
 </sst>
 </file>
 
@@ -1065,7 +1086,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1189,15 +1210,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1413,9 +1425,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1727,9 +1739,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1763,7 +1772,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1786,9 +1795,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1826,7 +1835,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1932,7 +1941,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2074,7 +2083,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2084,9 +2093,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE91C3C-F676-4E77-8227-802554E4B42D}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B10"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2184,7 +2193,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3:F12"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2289,7 +2298,9 @@
       <c r="E3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="118"/>
+      <c r="F3" s="117" t="s">
+        <v>340</v>
+      </c>
       <c r="G3" s="67" t="s">
         <v>7</v>
       </c>
@@ -2586,7 +2597,7 @@
       <c r="E12" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="119"/>
+      <c r="F12" s="118"/>
       <c r="G12" s="37" t="s">
         <v>7</v>
       </c>
@@ -2621,9 +2632,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5623B452-6320-41F9-A4C3-771E435FA050}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2722,7 +2733,9 @@
       <c r="E3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="67"/>
+      <c r="F3" s="67" t="s">
+        <v>342</v>
+      </c>
       <c r="G3" s="67" t="s">
         <v>7</v>
       </c>
@@ -3056,7 +3069,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3:F10"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3161,7 +3174,9 @@
       <c r="E3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="74"/>
+      <c r="F3" s="74" t="s">
+        <v>341</v>
+      </c>
       <c r="G3" s="67" t="s">
         <v>7</v>
       </c>
@@ -3453,7 +3468,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3542,7 +3557,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -3558,7 +3573,9 @@
       <c r="E3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="96"/>
+      <c r="F3" s="96" t="s">
+        <v>343</v>
+      </c>
       <c r="G3" s="67" t="s">
         <v>7</v>
       </c>
@@ -3786,7 +3803,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3:H24"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3889,9 +3906,15 @@
       <c r="E3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="76"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="68"/>
+      <c r="F3" s="76" t="s">
+        <v>344</v>
+      </c>
+      <c r="G3" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="68" t="s">
+        <v>7</v>
+      </c>
       <c r="I3" s="81" t="s">
         <v>7</v>
       </c>
@@ -4516,10 +4539,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8724B99-AD69-4DBF-8338-B0E3FE02CAE6}">
-  <dimension ref="A1:P87"/>
+  <dimension ref="A1:P86"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:G46"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4537,48 +4560,67 @@
     <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="107"/>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="1" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="94" t="s">
+      <c r="J1" s="94" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="82" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="87">
+        <v>50004</v>
+      </c>
+      <c r="J2" s="66" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>268</v>
+        <v>9</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>6</v>
@@ -4586,25 +4628,29 @@
       <c r="C3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="82" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="14"/>
+      <c r="D3" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>7</v>
+      </c>
       <c r="H3" s="15" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="87">
-        <v>50004</v>
-      </c>
-      <c r="J3" s="66" t="s">
-        <v>269</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="J3" s="66"/>
     </row>
     <row r="4" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>6</v>
@@ -4628,13 +4674,13 @@
         <v>7</v>
       </c>
       <c r="I4" s="87">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="J4" s="66"/>
     </row>
     <row r="5" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>6</v>
@@ -4658,13 +4704,13 @@
         <v>7</v>
       </c>
       <c r="I5" s="87">
-        <v>1</v>
+        <v>39035</v>
       </c>
       <c r="J5" s="66"/>
     </row>
     <row r="6" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>6</v>
@@ -4688,48 +4734,44 @@
         <v>7</v>
       </c>
       <c r="I6" s="87">
-        <v>39035</v>
-      </c>
-      <c r="J6" s="66"/>
+        <v>63</v>
+      </c>
+      <c r="J6" s="66" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="7" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>12</v>
+        <v>270</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="E7" s="36" t="s">
+        <v>339</v>
+      </c>
+      <c r="F7" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="87">
-        <v>63</v>
-      </c>
-      <c r="J7" s="66" t="s">
-        <v>223</v>
-      </c>
+      <c r="H7" s="15"/>
+      <c r="I7" s="107"/>
+      <c r="J7" s="66"/>
     </row>
     <row r="8" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>270</v>
+        <v>14</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>7</v>
@@ -4737,42 +4779,60 @@
       <c r="D8" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="83"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="108"/>
-      <c r="J8" s="66"/>
-    </row>
-    <row r="9" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="11" t="s">
+      <c r="E8" s="108" t="s">
+        <v>340</v>
+      </c>
+      <c r="F8" s="83" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="107" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="66" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="109"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="84"/>
+      <c r="E9" s="109" t="s">
+        <v>341</v>
+      </c>
+      <c r="F9" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="85" t="s">
+        <v>7</v>
+      </c>
       <c r="H9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="108" t="s">
+      <c r="I9" s="23" t="s">
         <v>7</v>
       </c>
       <c r="J9" s="66" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>122</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>15</v>
@@ -4783,9 +4843,15 @@
       <c r="D10" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="110"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="85"/>
+      <c r="E10" s="24" t="s">
+        <v>338</v>
+      </c>
+      <c r="F10" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="85" t="s">
+        <v>7</v>
+      </c>
       <c r="H10" s="15" t="s">
         <v>7</v>
       </c>
@@ -4793,25 +4859,31 @@
         <v>7</v>
       </c>
       <c r="J10" s="66" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B11" s="20" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="80"/>
-      <c r="G11" s="85"/>
+      <c r="E11" s="110" t="s">
+        <v>342</v>
+      </c>
+      <c r="F11" s="76" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="111" t="s">
+        <v>7</v>
+      </c>
       <c r="H11" s="15" t="s">
         <v>7</v>
       </c>
@@ -4819,47 +4891,47 @@
         <v>7</v>
       </c>
       <c r="J11" s="66" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="111"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="112"/>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="112" t="s">
+        <v>271</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="80"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="70"/>
       <c r="H12" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="23" t="s">
+      <c r="I12" s="87">
+        <v>5363</v>
+      </c>
+      <c r="J12" s="66" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="112" t="s">
+        <v>273</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="22" t="s">
         <v>7</v>
-      </c>
-      <c r="J12" s="66" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="113" t="s">
-        <v>271</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>10</v>
       </c>
       <c r="E13" s="80"/>
       <c r="F13" s="83"/>
@@ -4867,16 +4939,16 @@
       <c r="H13" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="87">
-        <v>5363</v>
+      <c r="I13" s="24" t="s">
+        <v>274</v>
       </c>
       <c r="J13" s="66" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="113" t="s">
-        <v>273</v>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="112" t="s">
+        <v>276</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>136</v>
@@ -4897,21 +4969,21 @@
         <v>274</v>
       </c>
       <c r="J14" s="66" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="113" t="s">
-        <v>276</v>
+      <c r="A15" s="112" t="s">
+        <v>278</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>136</v>
+        <v>25</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="22" t="s">
-        <v>7</v>
+      <c r="D15" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="E15" s="80"/>
       <c r="F15" s="83"/>
@@ -4919,25 +4991,25 @@
       <c r="H15" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="24" t="s">
-        <v>274</v>
+      <c r="I15" s="87" t="s">
+        <v>279</v>
       </c>
       <c r="J15" s="66" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="113" t="s">
-        <v>278</v>
+      <c r="A16" s="112" t="s">
+        <v>281</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="17" t="s">
-        <v>10</v>
+      <c r="D16" s="22" t="s">
+        <v>7</v>
       </c>
       <c r="E16" s="80"/>
       <c r="F16" s="83"/>
@@ -4945,19 +5017,19 @@
       <c r="H16" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="87" t="s">
-        <v>279</v>
+      <c r="I16" s="24" t="s">
+        <v>282</v>
       </c>
       <c r="J16" s="66" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="113" t="s">
-        <v>281</v>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="112" t="s">
+        <v>284</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>24</v>
@@ -4972,18 +5044,18 @@
         <v>7</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="J17" s="66" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="113" t="s">
-        <v>284</v>
+      <c r="A18" s="112" t="s">
+        <v>27</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>24</v>
@@ -4997,25 +5069,25 @@
       <c r="H18" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="24" t="s">
-        <v>285</v>
+      <c r="I18" s="23" t="s">
+        <v>7</v>
       </c>
       <c r="J18" s="66" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="113" t="s">
-        <v>27</v>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="112" t="s">
+        <v>287</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E19" s="80"/>
       <c r="F19" s="83"/>
@@ -5023,25 +5095,25 @@
       <c r="H19" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="23" t="s">
-        <v>7</v>
+      <c r="I19" s="24">
+        <v>5200</v>
       </c>
       <c r="J19" s="66" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="113" t="s">
-        <v>287</v>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="112" t="s">
+        <v>289</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E20" s="80"/>
       <c r="F20" s="83"/>
@@ -5050,24 +5122,24 @@
         <v>7</v>
       </c>
       <c r="I20" s="24">
-        <v>5200</v>
+        <v>1</v>
       </c>
       <c r="J20" s="66" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="113" t="s">
-        <v>289</v>
+      <c r="A21" s="112" t="s">
+        <v>291</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E21" s="80"/>
       <c r="F21" s="83"/>
@@ -5075,25 +5147,25 @@
       <c r="H21" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I21" s="24">
-        <v>1</v>
+      <c r="I21" s="24" t="s">
+        <v>292</v>
       </c>
       <c r="J21" s="66" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="113" t="s">
-        <v>291</v>
+        <v>293</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="112" t="s">
+        <v>294</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="12" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E22" s="80"/>
       <c r="F22" s="83"/>
@@ -5102,20 +5174,20 @@
         <v>7</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="J22" s="66" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="113" t="s">
-        <v>294</v>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="112" t="s">
+        <v>297</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="22" t="s">
@@ -5128,24 +5200,24 @@
         <v>7</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="J23" s="66" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="113" t="s">
-        <v>297</v>
+      <c r="A24" s="112" t="s">
+        <v>300</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>24</v>
+        <v>6</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>7</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E24" s="80"/>
       <c r="F24" s="83"/>
@@ -5154,24 +5226,24 @@
         <v>7</v>
       </c>
       <c r="I24" s="24" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="J24" s="66" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="113" t="s">
-        <v>300</v>
+        <v>302</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="112" t="s">
+        <v>303</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="22" t="s">
         <v>7</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>10</v>
       </c>
       <c r="E25" s="80"/>
       <c r="F25" s="83"/>
@@ -5179,16 +5251,16 @@
       <c r="H25" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I25" s="24" t="s">
-        <v>301</v>
+      <c r="I25" s="113">
+        <v>44196</v>
       </c>
       <c r="J25" s="66" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="113" t="s">
-        <v>303</v>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="112" t="s">
+        <v>306</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>304</v>
@@ -5205,25 +5277,25 @@
       <c r="H26" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I26" s="114">
-        <v>44196</v>
+      <c r="I26" s="113">
+        <v>43831</v>
       </c>
       <c r="J26" s="66" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="113" t="s">
-        <v>306</v>
+      <c r="A27" s="112" t="s">
+        <v>308</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>304</v>
+        <v>25</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E27" s="80"/>
       <c r="F27" s="83"/>
@@ -5231,25 +5303,25 @@
       <c r="H27" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I27" s="114">
-        <v>43831</v>
+      <c r="I27" s="24" t="s">
+        <v>274</v>
       </c>
       <c r="J27" s="66" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="113" t="s">
-        <v>308</v>
+      <c r="A28" s="112" t="s">
+        <v>310</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E28" s="80"/>
       <c r="F28" s="83"/>
@@ -5257,22 +5329,22 @@
       <c r="H28" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I28" s="24" t="s">
-        <v>274</v>
+      <c r="I28" s="24">
+        <v>0</v>
       </c>
       <c r="J28" s="66" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="113" t="s">
-        <v>310</v>
+      <c r="A29" s="55" t="s">
+        <v>141</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>7</v>
       </c>
       <c r="D29" s="22" t="s">
         <v>7</v>
@@ -5283,22 +5355,22 @@
       <c r="H29" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I29" s="24">
-        <v>0</v>
+      <c r="I29" s="23" t="s">
+        <v>7</v>
       </c>
       <c r="J29" s="66" t="s">
-        <v>311</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="55" t="s">
-        <v>141</v>
+      <c r="A30" s="112" t="s">
+        <v>28</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>7</v>
+      <c r="C30" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>7</v>
@@ -5309,25 +5381,25 @@
       <c r="H30" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I30" s="23" t="s">
-        <v>7</v>
+      <c r="I30" s="24" t="s">
+        <v>274</v>
       </c>
       <c r="J30" s="66" t="s">
-        <v>257</v>
+        <v>312</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="113" t="s">
-        <v>28</v>
+      <c r="A31" s="112" t="s">
+        <v>29</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E31" s="80"/>
       <c r="F31" s="83"/>
@@ -5339,12 +5411,12 @@
         <v>274</v>
       </c>
       <c r="J31" s="66" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="113" t="s">
-        <v>29</v>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="112" t="s">
+        <v>30</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>26</v>
@@ -5365,21 +5437,21 @@
         <v>274</v>
       </c>
       <c r="J32" s="66" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="113" t="s">
-        <v>30</v>
+        <v>314</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" s="112" t="s">
+        <v>315</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>7</v>
       </c>
       <c r="E33" s="80"/>
       <c r="F33" s="83"/>
@@ -5387,24 +5459,24 @@
       <c r="H33" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I33" s="24" t="s">
-        <v>274</v>
+      <c r="I33" s="114">
+        <v>43874</v>
       </c>
       <c r="J33" s="66" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A34" s="113" t="s">
-        <v>315</v>
+      <c r="A34" s="112" t="s">
+        <v>31</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="22" t="s">
         <v>7</v>
       </c>
       <c r="E34" s="80"/>
@@ -5414,18 +5486,18 @@
         <v>7</v>
       </c>
       <c r="I34" s="115">
-        <v>43874</v>
+        <v>33187</v>
       </c>
       <c r="J34" s="66" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A35" s="113" t="s">
-        <v>31</v>
+      <c r="A35" s="112" t="s">
+        <v>318</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>26</v>
+        <v>319</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>24</v>
@@ -5436,24 +5508,20 @@
       <c r="E35" s="80"/>
       <c r="F35" s="83"/>
       <c r="G35" s="70"/>
-      <c r="H35" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="I35" s="116">
-        <v>33187</v>
-      </c>
+      <c r="H35" s="15"/>
+      <c r="I35" s="115"/>
       <c r="J35" s="66" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A36" s="113" t="s">
-        <v>318</v>
+      <c r="A36" s="112" t="s">
+        <v>321</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="C36" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D36" s="22" t="s">
@@ -5462,15 +5530,19 @@
       <c r="E36" s="80"/>
       <c r="F36" s="83"/>
       <c r="G36" s="70"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="116"/>
+      <c r="H36" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="23" t="s">
+        <v>7</v>
+      </c>
       <c r="J36" s="66" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A37" s="113" t="s">
-        <v>321</v>
+      <c r="A37" s="112" t="s">
+        <v>33</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>23</v>
@@ -5484,52 +5556,52 @@
       <c r="E37" s="80"/>
       <c r="F37" s="83"/>
       <c r="G37" s="70"/>
-      <c r="H37" s="15" t="s">
-        <v>7</v>
-      </c>
+      <c r="H37" s="28"/>
       <c r="I37" s="23" t="s">
         <v>7</v>
       </c>
       <c r="J37" s="66" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A38" s="113" t="s">
-        <v>33</v>
+      <c r="A38" s="112" t="s">
+        <v>35</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C38" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E38" s="80"/>
       <c r="F38" s="83"/>
       <c r="G38" s="70"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="23" t="s">
+      <c r="H38" s="15" t="s">
         <v>7</v>
       </c>
+      <c r="I38" s="24" t="s">
+        <v>274</v>
+      </c>
       <c r="J38" s="66" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A39" s="113" t="s">
-        <v>35</v>
+      <c r="A39" s="112" t="s">
+        <v>325</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E39" s="80"/>
       <c r="F39" s="83"/>
@@ -5537,16 +5609,16 @@
       <c r="H39" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I39" s="24" t="s">
-        <v>274</v>
+      <c r="I39" s="23" t="s">
+        <v>7</v>
       </c>
       <c r="J39" s="66" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A40" s="113" t="s">
-        <v>325</v>
+        <v>326</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="10" t="s">
+        <v>327</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>25</v>
@@ -5554,8 +5626,8 @@
       <c r="C40" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D40" s="22" t="s">
-        <v>7</v>
+      <c r="D40" s="31" t="s">
+        <v>10</v>
       </c>
       <c r="E40" s="80"/>
       <c r="F40" s="83"/>
@@ -5564,24 +5636,30 @@
         <v>7</v>
       </c>
       <c r="I40" s="23" t="s">
-        <v>7</v>
+        <v>328</v>
       </c>
       <c r="J40" s="66" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="10" t="s">
-        <v>327</v>
+        <v>329</v>
+      </c>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A41" s="112" t="s">
+        <v>36</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="31" t="s">
-        <v>10</v>
+      <c r="D41" s="22" t="s">
+        <v>7</v>
       </c>
       <c r="E41" s="80"/>
       <c r="F41" s="83"/>
@@ -5590,30 +5668,24 @@
         <v>7</v>
       </c>
       <c r="I41" s="23" t="s">
-        <v>328</v>
+        <v>7</v>
       </c>
       <c r="J41" s="66" t="s">
-        <v>329</v>
-      </c>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
+        <v>330</v>
+      </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A42" s="113" t="s">
-        <v>36</v>
+      <c r="A42" s="112" t="s">
+        <v>37</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="C42" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D42" s="22" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E42" s="80"/>
       <c r="F42" s="83"/>
@@ -5621,24 +5693,28 @@
       <c r="H42" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I42" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="J42" s="66" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A43" s="113" t="s">
-        <v>37</v>
+      <c r="I42" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="J42" s="66"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+    </row>
+    <row r="43" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="112" t="s">
+        <v>331</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D43" s="22" t="s">
+      <c r="D43" s="17" t="s">
         <v>10</v>
       </c>
       <c r="E43" s="80"/>
@@ -5647,20 +5723,22 @@
       <c r="H43" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="24" t="s">
-        <v>274</v>
-      </c>
-      <c r="J43" s="66"/>
-      <c r="K43" s="10"/>
-      <c r="L43" s="10"/>
-      <c r="M43" s="10"/>
-      <c r="N43" s="10"/>
-      <c r="O43" s="10"/>
-      <c r="P43" s="10"/>
-    </row>
-    <row r="44" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="113" t="s">
-        <v>331</v>
+      <c r="I43" s="87" t="s">
+        <v>332</v>
+      </c>
+      <c r="J43" s="66" t="s">
+        <v>333</v>
+      </c>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A44" s="112" t="s">
+        <v>334</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>26</v>
@@ -5674,75 +5752,48 @@
       <c r="E44" s="80"/>
       <c r="F44" s="83"/>
       <c r="G44" s="70"/>
-      <c r="H44" s="15" t="s">
+      <c r="H44" s="116"/>
+      <c r="I44" s="87"/>
+      <c r="J44" s="66" t="s">
+        <v>335</v>
+      </c>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A45" s="112" t="s">
+        <v>336</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D45" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I44" s="87" t="s">
-        <v>332</v>
-      </c>
-      <c r="J44" s="66" t="s">
-        <v>333</v>
-      </c>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A45" s="113" t="s">
-        <v>334</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E45" s="80"/>
+      <c r="E45" s="83"/>
       <c r="F45" s="83"/>
-      <c r="G45" s="70"/>
-      <c r="H45" s="117"/>
-      <c r="I45" s="87"/>
+      <c r="G45" s="59"/>
+      <c r="H45" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" s="24" t="s">
+        <v>274</v>
+      </c>
       <c r="J45" s="66" t="s">
-        <v>335</v>
-      </c>
-      <c r="K45" s="10"/>
-      <c r="L45" s="10"/>
-      <c r="M45" s="10"/>
-      <c r="N45" s="10"/>
-      <c r="O45" s="10"/>
-      <c r="P45" s="10"/>
+        <v>337</v>
+      </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A46" s="113" t="s">
-        <v>336</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D46" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" s="83"/>
-      <c r="F46" s="83"/>
-      <c r="G46" s="59"/>
-      <c r="H46" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="I46" s="24" t="s">
-        <v>274</v>
-      </c>
-      <c r="J46" s="66" t="s">
-        <v>337</v>
-      </c>
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="10"/>
@@ -5759,13 +5810,8 @@
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="64"/>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" s="64"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -55957,7 +56003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A26DA6-FFEA-403F-8C16-B9588EA712AA}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>

</xml_diff>